<commit_message>
improvment of the 2d model called "PCM_model". no calibration working.
</commit_message>
<xml_diff>
--- a/data/h(T)_2.xlsx
+++ b/data/h(T)_2.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\ginevra.licastri\Desktop\Python Projects\PCM_AIR_HEX_2D\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F64742C2-7985-4733-A819-5F5D615F2CD3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{39F45C8D-5C79-45E2-95C1-597B05A169E2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-109" yWindow="-109" windowWidth="26301" windowHeight="14169" xr2:uid="{A50B25A9-7068-403E-BF10-45ACB44710EA}"/>
   </bookViews>
@@ -468,130 +468,130 @@
                   <c:v>36000</c:v>
                 </c:pt>
                 <c:pt idx="23">
-                  <c:v>96000</c:v>
+                  <c:v>106000</c:v>
                 </c:pt>
                 <c:pt idx="24">
-                  <c:v>156000</c:v>
+                  <c:v>176000</c:v>
                 </c:pt>
                 <c:pt idx="25">
-                  <c:v>216000</c:v>
+                  <c:v>246000</c:v>
                 </c:pt>
                 <c:pt idx="26">
-                  <c:v>276000</c:v>
+                  <c:v>316000</c:v>
                 </c:pt>
                 <c:pt idx="27">
-                  <c:v>278000</c:v>
+                  <c:v>318000</c:v>
                 </c:pt>
                 <c:pt idx="28">
-                  <c:v>280000</c:v>
+                  <c:v>320000</c:v>
                 </c:pt>
                 <c:pt idx="29">
-                  <c:v>282000</c:v>
+                  <c:v>322000</c:v>
                 </c:pt>
                 <c:pt idx="30">
-                  <c:v>284000</c:v>
+                  <c:v>324000</c:v>
                 </c:pt>
                 <c:pt idx="31">
-                  <c:v>286000</c:v>
+                  <c:v>326000</c:v>
                 </c:pt>
                 <c:pt idx="32">
-                  <c:v>288000</c:v>
+                  <c:v>328000</c:v>
                 </c:pt>
                 <c:pt idx="33">
-                  <c:v>290000</c:v>
+                  <c:v>330000</c:v>
                 </c:pt>
                 <c:pt idx="34">
-                  <c:v>292000</c:v>
+                  <c:v>332000</c:v>
                 </c:pt>
                 <c:pt idx="35">
-                  <c:v>294000</c:v>
+                  <c:v>334000</c:v>
                 </c:pt>
                 <c:pt idx="36">
-                  <c:v>296000</c:v>
+                  <c:v>336000</c:v>
                 </c:pt>
                 <c:pt idx="37">
-                  <c:v>298000</c:v>
+                  <c:v>338000</c:v>
                 </c:pt>
                 <c:pt idx="38">
-                  <c:v>300000</c:v>
+                  <c:v>340000</c:v>
                 </c:pt>
                 <c:pt idx="39">
-                  <c:v>302000</c:v>
+                  <c:v>342000</c:v>
                 </c:pt>
                 <c:pt idx="40">
-                  <c:v>304000</c:v>
+                  <c:v>344000</c:v>
                 </c:pt>
                 <c:pt idx="41">
-                  <c:v>306000</c:v>
+                  <c:v>346000</c:v>
                 </c:pt>
                 <c:pt idx="42">
-                  <c:v>308000</c:v>
+                  <c:v>348000</c:v>
                 </c:pt>
                 <c:pt idx="43">
-                  <c:v>310000</c:v>
+                  <c:v>350000</c:v>
                 </c:pt>
                 <c:pt idx="44">
-                  <c:v>312000</c:v>
+                  <c:v>352000</c:v>
                 </c:pt>
                 <c:pt idx="45">
-                  <c:v>314000</c:v>
+                  <c:v>354000</c:v>
                 </c:pt>
                 <c:pt idx="46">
-                  <c:v>316000</c:v>
+                  <c:v>356000</c:v>
                 </c:pt>
                 <c:pt idx="47">
-                  <c:v>318000</c:v>
+                  <c:v>358000</c:v>
                 </c:pt>
                 <c:pt idx="48">
-                  <c:v>320000</c:v>
+                  <c:v>360000</c:v>
                 </c:pt>
                 <c:pt idx="49">
-                  <c:v>322000</c:v>
+                  <c:v>362000</c:v>
                 </c:pt>
                 <c:pt idx="50">
-                  <c:v>324000</c:v>
+                  <c:v>364000</c:v>
                 </c:pt>
                 <c:pt idx="51">
-                  <c:v>326000</c:v>
+                  <c:v>366000</c:v>
                 </c:pt>
                 <c:pt idx="52">
-                  <c:v>328000</c:v>
+                  <c:v>368000</c:v>
                 </c:pt>
                 <c:pt idx="53">
-                  <c:v>330000</c:v>
+                  <c:v>370000</c:v>
                 </c:pt>
                 <c:pt idx="54">
-                  <c:v>332000</c:v>
+                  <c:v>372000</c:v>
                 </c:pt>
                 <c:pt idx="55">
-                  <c:v>334000</c:v>
+                  <c:v>374000</c:v>
                 </c:pt>
                 <c:pt idx="56">
-                  <c:v>336000</c:v>
+                  <c:v>376000</c:v>
                 </c:pt>
                 <c:pt idx="57">
-                  <c:v>338000</c:v>
+                  <c:v>378000</c:v>
                 </c:pt>
                 <c:pt idx="58">
-                  <c:v>340000</c:v>
+                  <c:v>380000</c:v>
                 </c:pt>
                 <c:pt idx="59">
-                  <c:v>342000</c:v>
+                  <c:v>382000</c:v>
                 </c:pt>
                 <c:pt idx="60">
-                  <c:v>344000</c:v>
+                  <c:v>384000</c:v>
                 </c:pt>
                 <c:pt idx="61">
-                  <c:v>346000</c:v>
+                  <c:v>386000</c:v>
                 </c:pt>
                 <c:pt idx="62">
-                  <c:v>348000</c:v>
+                  <c:v>388000</c:v>
                 </c:pt>
                 <c:pt idx="63">
-                  <c:v>350000</c:v>
+                  <c:v>390000</c:v>
                 </c:pt>
                 <c:pt idx="64">
-                  <c:v>352000</c:v>
+                  <c:v>392000</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -829,130 +829,130 @@
                   <c:v>36000</c:v>
                 </c:pt>
                 <c:pt idx="23">
-                  <c:v>96000</c:v>
+                  <c:v>106000</c:v>
                 </c:pt>
                 <c:pt idx="24">
-                  <c:v>156000</c:v>
+                  <c:v>176000</c:v>
                 </c:pt>
                 <c:pt idx="25">
-                  <c:v>216000</c:v>
+                  <c:v>246000</c:v>
                 </c:pt>
                 <c:pt idx="26">
-                  <c:v>276000</c:v>
+                  <c:v>316000</c:v>
                 </c:pt>
                 <c:pt idx="27">
-                  <c:v>278000</c:v>
+                  <c:v>318000</c:v>
                 </c:pt>
                 <c:pt idx="28">
-                  <c:v>280000</c:v>
+                  <c:v>320000</c:v>
                 </c:pt>
                 <c:pt idx="29">
-                  <c:v>282000</c:v>
+                  <c:v>322000</c:v>
                 </c:pt>
                 <c:pt idx="30">
-                  <c:v>284000</c:v>
+                  <c:v>324000</c:v>
                 </c:pt>
                 <c:pt idx="31">
-                  <c:v>286000</c:v>
+                  <c:v>326000</c:v>
                 </c:pt>
                 <c:pt idx="32">
-                  <c:v>288000</c:v>
+                  <c:v>328000</c:v>
                 </c:pt>
                 <c:pt idx="33">
-                  <c:v>290000</c:v>
+                  <c:v>330000</c:v>
                 </c:pt>
                 <c:pt idx="34">
-                  <c:v>292000</c:v>
+                  <c:v>332000</c:v>
                 </c:pt>
                 <c:pt idx="35">
-                  <c:v>294000</c:v>
+                  <c:v>334000</c:v>
                 </c:pt>
                 <c:pt idx="36">
-                  <c:v>296000</c:v>
+                  <c:v>336000</c:v>
                 </c:pt>
                 <c:pt idx="37">
-                  <c:v>298000</c:v>
+                  <c:v>338000</c:v>
                 </c:pt>
                 <c:pt idx="38">
-                  <c:v>300000</c:v>
+                  <c:v>340000</c:v>
                 </c:pt>
                 <c:pt idx="39">
-                  <c:v>302000</c:v>
+                  <c:v>342000</c:v>
                 </c:pt>
                 <c:pt idx="40">
-                  <c:v>304000</c:v>
+                  <c:v>344000</c:v>
                 </c:pt>
                 <c:pt idx="41">
-                  <c:v>306000</c:v>
+                  <c:v>346000</c:v>
                 </c:pt>
                 <c:pt idx="42">
-                  <c:v>308000</c:v>
+                  <c:v>348000</c:v>
                 </c:pt>
                 <c:pt idx="43">
-                  <c:v>310000</c:v>
+                  <c:v>350000</c:v>
                 </c:pt>
                 <c:pt idx="44">
-                  <c:v>312000</c:v>
+                  <c:v>352000</c:v>
                 </c:pt>
                 <c:pt idx="45">
-                  <c:v>314000</c:v>
+                  <c:v>354000</c:v>
                 </c:pt>
                 <c:pt idx="46">
-                  <c:v>316000</c:v>
+                  <c:v>356000</c:v>
                 </c:pt>
                 <c:pt idx="47">
-                  <c:v>318000</c:v>
+                  <c:v>358000</c:v>
                 </c:pt>
                 <c:pt idx="48">
-                  <c:v>320000</c:v>
+                  <c:v>360000</c:v>
                 </c:pt>
                 <c:pt idx="49">
-                  <c:v>322000</c:v>
+                  <c:v>362000</c:v>
                 </c:pt>
                 <c:pt idx="50">
-                  <c:v>324000</c:v>
+                  <c:v>364000</c:v>
                 </c:pt>
                 <c:pt idx="51">
-                  <c:v>326000</c:v>
+                  <c:v>366000</c:v>
                 </c:pt>
                 <c:pt idx="52">
-                  <c:v>328000</c:v>
+                  <c:v>368000</c:v>
                 </c:pt>
                 <c:pt idx="53">
-                  <c:v>330000</c:v>
+                  <c:v>370000</c:v>
                 </c:pt>
                 <c:pt idx="54">
-                  <c:v>332000</c:v>
+                  <c:v>372000</c:v>
                 </c:pt>
                 <c:pt idx="55">
-                  <c:v>334000</c:v>
+                  <c:v>374000</c:v>
                 </c:pt>
                 <c:pt idx="56">
-                  <c:v>336000</c:v>
+                  <c:v>376000</c:v>
                 </c:pt>
                 <c:pt idx="57">
-                  <c:v>338000</c:v>
+                  <c:v>378000</c:v>
                 </c:pt>
                 <c:pt idx="58">
-                  <c:v>340000</c:v>
+                  <c:v>380000</c:v>
                 </c:pt>
                 <c:pt idx="59">
-                  <c:v>342000</c:v>
+                  <c:v>382000</c:v>
                 </c:pt>
                 <c:pt idx="60">
-                  <c:v>344000</c:v>
+                  <c:v>384000</c:v>
                 </c:pt>
                 <c:pt idx="61">
-                  <c:v>346000</c:v>
+                  <c:v>386000</c:v>
                 </c:pt>
                 <c:pt idx="62">
-                  <c:v>348000</c:v>
+                  <c:v>388000</c:v>
                 </c:pt>
                 <c:pt idx="63">
-                  <c:v>350000</c:v>
+                  <c:v>390000</c:v>
                 </c:pt>
                 <c:pt idx="64">
-                  <c:v>352000</c:v>
+                  <c:v>392000</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -1691,8 +1691,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{DE06A95B-2A49-4267-873D-89653E918AAA}">
   <dimension ref="A1:G66"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A12" workbookViewId="0">
-      <selection activeCell="B26" sqref="B26"/>
+    <sheetView tabSelected="1" topLeftCell="A9" workbookViewId="0">
+      <selection activeCell="D34" sqref="D34"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.3" x14ac:dyDescent="0.25"/>
@@ -1719,7 +1719,7 @@
         <v>-4</v>
       </c>
       <c r="B2">
-        <f t="shared" ref="B2:B24" si="0">$F$1*(A2-$A$6)</f>
+        <f t="shared" ref="B2:B23" si="0">$F$1*(A2-$A$6)</f>
         <v>-8000</v>
       </c>
       <c r="E2" t="s">
@@ -1936,7 +1936,7 @@
       </c>
       <c r="B25">
         <f>B24+D34*(A26-A25)</f>
-        <v>96000</v>
+        <v>106000</v>
       </c>
     </row>
     <row r="26" spans="1:2" x14ac:dyDescent="0.25">
@@ -1945,7 +1945,7 @@
       </c>
       <c r="B26">
         <f>B25+D34*(A27-A26)</f>
-        <v>156000</v>
+        <v>176000</v>
       </c>
     </row>
     <row r="27" spans="1:2" x14ac:dyDescent="0.25">
@@ -1954,7 +1954,7 @@
       </c>
       <c r="B27">
         <f>B26+D34*(A28-A27)</f>
-        <v>216000</v>
+        <v>246000</v>
       </c>
     </row>
     <row r="28" spans="1:2" x14ac:dyDescent="0.25">
@@ -1963,7 +1963,7 @@
       </c>
       <c r="B28">
         <f>B27+D34*(A34-A33)</f>
-        <v>276000</v>
+        <v>316000</v>
       </c>
     </row>
     <row r="29" spans="1:2" x14ac:dyDescent="0.25">
@@ -1972,7 +1972,7 @@
       </c>
       <c r="B29">
         <f>B28+$F$2*(A29-A28)</f>
-        <v>278000</v>
+        <v>318000</v>
       </c>
     </row>
     <row r="30" spans="1:2" x14ac:dyDescent="0.25">
@@ -1980,8 +1980,8 @@
         <v>24</v>
       </c>
       <c r="B30">
-        <f t="shared" ref="B30:B36" si="1">B29+$F$2*(A30-A29)</f>
-        <v>280000</v>
+        <f>B29+$F$2*(A30-A29)</f>
+        <v>320000</v>
       </c>
     </row>
     <row r="31" spans="1:2" x14ac:dyDescent="0.25">
@@ -1989,8 +1989,8 @@
         <v>25</v>
       </c>
       <c r="B31">
-        <f t="shared" si="1"/>
-        <v>282000</v>
+        <f t="shared" ref="B30:B36" si="1">B30+$F$2*(A31-A30)</f>
+        <v>322000</v>
       </c>
     </row>
     <row r="32" spans="1:2" x14ac:dyDescent="0.25">
@@ -1999,7 +1999,7 @@
       </c>
       <c r="B32">
         <f t="shared" si="1"/>
-        <v>284000</v>
+        <v>324000</v>
       </c>
     </row>
     <row r="33" spans="1:4" x14ac:dyDescent="0.25">
@@ -2008,7 +2008,7 @@
       </c>
       <c r="B33">
         <f t="shared" si="1"/>
-        <v>286000</v>
+        <v>326000</v>
       </c>
     </row>
     <row r="34" spans="1:4" x14ac:dyDescent="0.25">
@@ -2017,10 +2017,10 @@
       </c>
       <c r="B34">
         <f t="shared" si="1"/>
-        <v>288000</v>
+        <v>328000</v>
       </c>
       <c r="D34">
-        <v>60000</v>
+        <v>70000</v>
       </c>
     </row>
     <row r="35" spans="1:4" x14ac:dyDescent="0.25">
@@ -2029,7 +2029,7 @@
       </c>
       <c r="B35">
         <f t="shared" si="1"/>
-        <v>290000</v>
+        <v>330000</v>
       </c>
     </row>
     <row r="36" spans="1:4" x14ac:dyDescent="0.25">
@@ -2038,7 +2038,7 @@
       </c>
       <c r="B36">
         <f t="shared" si="1"/>
-        <v>292000</v>
+        <v>332000</v>
       </c>
     </row>
     <row r="37" spans="1:4" x14ac:dyDescent="0.25">
@@ -2047,7 +2047,7 @@
       </c>
       <c r="B37">
         <f>B36+$F$2*(A37-A36)</f>
-        <v>294000</v>
+        <v>334000</v>
       </c>
     </row>
     <row r="38" spans="1:4" x14ac:dyDescent="0.25">
@@ -2056,7 +2056,7 @@
       </c>
       <c r="B38">
         <f t="shared" ref="B38:B66" si="2">B37+$F$2*(A38-A37)</f>
-        <v>296000</v>
+        <v>336000</v>
       </c>
     </row>
     <row r="39" spans="1:4" x14ac:dyDescent="0.25">
@@ -2065,7 +2065,7 @@
       </c>
       <c r="B39">
         <f t="shared" si="2"/>
-        <v>298000</v>
+        <v>338000</v>
       </c>
     </row>
     <row r="40" spans="1:4" x14ac:dyDescent="0.25">
@@ -2074,7 +2074,7 @@
       </c>
       <c r="B40">
         <f>B39+$F$2*(A40-A39)</f>
-        <v>300000</v>
+        <v>340000</v>
       </c>
     </row>
     <row r="41" spans="1:4" x14ac:dyDescent="0.25">
@@ -2083,7 +2083,7 @@
       </c>
       <c r="B41">
         <f t="shared" si="2"/>
-        <v>302000</v>
+        <v>342000</v>
       </c>
     </row>
     <row r="42" spans="1:4" x14ac:dyDescent="0.25">
@@ -2092,7 +2092,7 @@
       </c>
       <c r="B42">
         <f t="shared" si="2"/>
-        <v>304000</v>
+        <v>344000</v>
       </c>
     </row>
     <row r="43" spans="1:4" x14ac:dyDescent="0.25">
@@ -2101,7 +2101,7 @@
       </c>
       <c r="B43">
         <f t="shared" si="2"/>
-        <v>306000</v>
+        <v>346000</v>
       </c>
     </row>
     <row r="44" spans="1:4" x14ac:dyDescent="0.25">
@@ -2110,7 +2110,7 @@
       </c>
       <c r="B44">
         <f t="shared" si="2"/>
-        <v>308000</v>
+        <v>348000</v>
       </c>
     </row>
     <row r="45" spans="1:4" x14ac:dyDescent="0.25">
@@ -2119,7 +2119,7 @@
       </c>
       <c r="B45">
         <f t="shared" si="2"/>
-        <v>310000</v>
+        <v>350000</v>
       </c>
     </row>
     <row r="46" spans="1:4" x14ac:dyDescent="0.25">
@@ -2128,7 +2128,7 @@
       </c>
       <c r="B46">
         <f t="shared" si="2"/>
-        <v>312000</v>
+        <v>352000</v>
       </c>
     </row>
     <row r="47" spans="1:4" x14ac:dyDescent="0.25">
@@ -2137,7 +2137,7 @@
       </c>
       <c r="B47">
         <f t="shared" si="2"/>
-        <v>314000</v>
+        <v>354000</v>
       </c>
     </row>
     <row r="48" spans="1:4" x14ac:dyDescent="0.25">
@@ -2146,7 +2146,7 @@
       </c>
       <c r="B48">
         <f t="shared" si="2"/>
-        <v>316000</v>
+        <v>356000</v>
       </c>
     </row>
     <row r="49" spans="1:2" x14ac:dyDescent="0.25">
@@ -2155,7 +2155,7 @@
       </c>
       <c r="B49">
         <f t="shared" si="2"/>
-        <v>318000</v>
+        <v>358000</v>
       </c>
     </row>
     <row r="50" spans="1:2" x14ac:dyDescent="0.25">
@@ -2164,7 +2164,7 @@
       </c>
       <c r="B50">
         <f t="shared" si="2"/>
-        <v>320000</v>
+        <v>360000</v>
       </c>
     </row>
     <row r="51" spans="1:2" x14ac:dyDescent="0.25">
@@ -2173,7 +2173,7 @@
       </c>
       <c r="B51">
         <f t="shared" si="2"/>
-        <v>322000</v>
+        <v>362000</v>
       </c>
     </row>
     <row r="52" spans="1:2" x14ac:dyDescent="0.25">
@@ -2182,7 +2182,7 @@
       </c>
       <c r="B52">
         <f t="shared" si="2"/>
-        <v>324000</v>
+        <v>364000</v>
       </c>
     </row>
     <row r="53" spans="1:2" x14ac:dyDescent="0.25">
@@ -2191,7 +2191,7 @@
       </c>
       <c r="B53">
         <f t="shared" si="2"/>
-        <v>326000</v>
+        <v>366000</v>
       </c>
     </row>
     <row r="54" spans="1:2" x14ac:dyDescent="0.25">
@@ -2200,7 +2200,7 @@
       </c>
       <c r="B54">
         <f t="shared" si="2"/>
-        <v>328000</v>
+        <v>368000</v>
       </c>
     </row>
     <row r="55" spans="1:2" x14ac:dyDescent="0.25">
@@ -2209,7 +2209,7 @@
       </c>
       <c r="B55">
         <f t="shared" si="2"/>
-        <v>330000</v>
+        <v>370000</v>
       </c>
     </row>
     <row r="56" spans="1:2" x14ac:dyDescent="0.25">
@@ -2218,7 +2218,7 @@
       </c>
       <c r="B56">
         <f t="shared" si="2"/>
-        <v>332000</v>
+        <v>372000</v>
       </c>
     </row>
     <row r="57" spans="1:2" x14ac:dyDescent="0.25">
@@ -2227,7 +2227,7 @@
       </c>
       <c r="B57">
         <f t="shared" si="2"/>
-        <v>334000</v>
+        <v>374000</v>
       </c>
     </row>
     <row r="58" spans="1:2" x14ac:dyDescent="0.25">
@@ -2236,7 +2236,7 @@
       </c>
       <c r="B58">
         <f t="shared" si="2"/>
-        <v>336000</v>
+        <v>376000</v>
       </c>
     </row>
     <row r="59" spans="1:2" x14ac:dyDescent="0.25">
@@ -2245,7 +2245,7 @@
       </c>
       <c r="B59">
         <f t="shared" si="2"/>
-        <v>338000</v>
+        <v>378000</v>
       </c>
     </row>
     <row r="60" spans="1:2" x14ac:dyDescent="0.25">
@@ -2254,7 +2254,7 @@
       </c>
       <c r="B60">
         <f t="shared" si="2"/>
-        <v>340000</v>
+        <v>380000</v>
       </c>
     </row>
     <row r="61" spans="1:2" x14ac:dyDescent="0.25">
@@ -2263,7 +2263,7 @@
       </c>
       <c r="B61">
         <f t="shared" si="2"/>
-        <v>342000</v>
+        <v>382000</v>
       </c>
     </row>
     <row r="62" spans="1:2" x14ac:dyDescent="0.25">
@@ -2272,7 +2272,7 @@
       </c>
       <c r="B62">
         <f t="shared" si="2"/>
-        <v>344000</v>
+        <v>384000</v>
       </c>
     </row>
     <row r="63" spans="1:2" x14ac:dyDescent="0.25">
@@ -2281,7 +2281,7 @@
       </c>
       <c r="B63">
         <f t="shared" si="2"/>
-        <v>346000</v>
+        <v>386000</v>
       </c>
     </row>
     <row r="64" spans="1:2" x14ac:dyDescent="0.25">
@@ -2290,7 +2290,7 @@
       </c>
       <c r="B64">
         <f t="shared" si="2"/>
-        <v>348000</v>
+        <v>388000</v>
       </c>
     </row>
     <row r="65" spans="1:2" x14ac:dyDescent="0.25">
@@ -2299,7 +2299,7 @@
       </c>
       <c r="B65">
         <f t="shared" si="2"/>
-        <v>350000</v>
+        <v>390000</v>
       </c>
     </row>
     <row r="66" spans="1:2" x14ac:dyDescent="0.25">
@@ -2308,7 +2308,7 @@
       </c>
       <c r="B66">
         <f t="shared" si="2"/>
-        <v>352000</v>
+        <v>392000</v>
       </c>
     </row>
   </sheetData>

</xml_diff>